<commit_message>
Caricata la II Pietro e parte della I Pietro
Caricata parte della I Lettera di San Pietro Apostolo (1 Pt o 1Pt o I Pt o Petri I o 1Ptr)
Caricata tutta la II Lettera di San Pietro Aapostolo (2 Pt o 2Pt o II Pt o Petri II o 2Ptr)
</commit_message>
<xml_diff>
--- a/1Gv3.xlsx
+++ b/1Gv3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="Questa_cartella_di_lavoro" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documenti\GitHub\EmanueleTinari\La-Sacra-Bibbia-In-Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD002DF-621C-4495-9659-BABEB456F4E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E49A00B-8C0D-4CEC-8DAD-F9AAEF7650A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="761" activeTab="12" xr2:uid="{D986225B-B090-490E-B2D4-FD06F5AD3E78}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="761" xr2:uid="{D986225B-B090-490E-B2D4-FD06F5AD3E78}"/>
   </bookViews>
   <sheets>
     <sheet name="1Gv3-VLSG" sheetId="1" r:id="rId1"/>
@@ -1645,7 +1645,7 @@
   </sheetPr>
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23" x14ac:dyDescent="0.5"/>
   <cols>
@@ -2652,7 +2652,7 @@
   </sheetPr>
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23" x14ac:dyDescent="0.5"/>
   <cols>

</xml_diff>